<commit_message>
Update countries & provincias Spain
</commit_message>
<xml_diff>
--- a/countries.xlsx
+++ b/countries.xlsx
@@ -571,7 +571,7 @@
     <t>Nepal</t>
   </si>
   <si>
-    <t>Datos actualizados a 19 de Marzo de 2020 a las 20:29</t>
+    <t>Datos actualizados a 19 de Marzo de 2020 a las 20:34</t>
   </si>
 </sst>
 </file>
@@ -1068,25 +1068,25 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>17395</v>
+        <v>17963</v>
       </c>
       <c r="C7">
-        <v>2626</v>
+        <v>3194</v>
       </c>
       <c r="D7">
         <v>1107</v>
       </c>
       <c r="E7">
-        <v>15485</v>
+        <v>16026</v>
       </c>
       <c r="F7">
         <v>800</v>
       </c>
       <c r="G7">
-        <v>165</v>
+        <v>192</v>
       </c>
       <c r="H7">
-        <v>803</v>
+        <v>830</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1120,16 +1120,16 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>11432</v>
+        <v>11597</v>
       </c>
       <c r="C9">
-        <v>2173</v>
+        <v>2338</v>
       </c>
       <c r="D9">
         <v>108</v>
       </c>
       <c r="E9">
-        <v>11153</v>
+        <v>11318</v>
       </c>
       <c r="F9">
         <v>64</v>

</xml_diff>